<commit_message>
Updated one of the example templates
</commit_message>
<xml_diff>
--- a/batch_template_JHT2.xlsx
+++ b/batch_template_JHT2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coverney\Documents\SynBio\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coverney\Documents\GitHub\TASBEFlowAnalytics-Tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-40860" yWindow="2835" windowWidth="28035" windowHeight="15945"/>
+    <workbookView xWindow="-40860" yWindow="2835" windowWidth="28035" windowHeight="15945" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="268">
   <si>
     <t>AF01</t>
   </si>
@@ -837,7 +837,10 @@
     <t>1_2_3_4_5.fcs</t>
   </si>
   <si>
-    <t>C:/Users/coverney/Documents/GitHub/TASBEFlowAnalytics-Tutorial</t>
+    <t>Template #</t>
+  </si>
+  <si>
+    <t>input filepath</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1053,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1438,17 +1441,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -1476,7 +1468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1757,17 +1749,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1780,6 +1769,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1896,6 +1888,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2213,8 +2208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2341,7 +2336,7 @@
       <c r="F12" s="118"/>
       <c r="G12" s="118"/>
       <c r="H12" s="119"/>
-      <c r="J12" s="110" t="s">
+      <c r="J12" s="109" t="s">
         <v>247</v>
       </c>
     </row>
@@ -2362,7 +2357,7 @@
         <v>240</v>
       </c>
       <c r="J13" s="116" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2597,7 +2592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -2937,7 +2932,7 @@
       <c r="C18" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="D18" s="113" t="s">
+      <c r="D18" s="112" t="s">
         <v>167</v>
       </c>
       <c r="F18" s="87"/>
@@ -2996,7 +2991,7 @@
       <c r="J21" s="97"/>
     </row>
     <row r="22" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="114" t="s">
+      <c r="A22" s="113" t="s">
         <v>264</v>
       </c>
       <c r="B22" s="50" t="str">
@@ -3043,10 +3038,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3102,8 +3097,8 @@
       <c r="G2" s="31">
         <v>6</v>
       </c>
-      <c r="H2" s="31">
-        <v>7</v>
+      <c r="H2" s="115" t="s">
+        <v>266</v>
       </c>
       <c r="I2" s="31">
         <v>8</v>
@@ -3147,27 +3142,20 @@
         <v>23</v>
       </c>
       <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="H3" s="37">
+        <v>1</v>
+      </c>
       <c r="I3" s="37"/>
       <c r="J3" s="38" t="s">
         <v>46</v>
       </c>
       <c r="K3" s="39" t="str">
-        <f>CONCATENATE(B3,CHAR(13),C3,CHAR(13),D3,CHAR(13),E3,CHAR(13),F3,CHAR(13),G3,CHAR(13),H3,CHAR(13),I3)</f>
-        <v>X_x000D_No_x000D_-_x000D_-_x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L3" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J3, SEARCH(",", J3, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_A1.fcs</v>
-      </c>
-      <c r="M3" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J3, SEARCH(",",J3) + 1, SEARCH(",",J3,SEARCH(",",J3)+1) - SEARCH(",",J3) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_A2.fcs</v>
-      </c>
-      <c r="N3" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J3,LEN(J3) - SEARCH(",", J3, SEARCH(",", J3) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_A3.fcs</v>
-      </c>
+        <f>CONCATENATE(B3,CHAR(13),C3,CHAR(13),D3,CHAR(13),E3,CHAR(13),F3)</f>
+        <v>X_x000D_No_x000D_-_x000D_-_x000D_6 hrs</v>
+      </c>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
       <c r="O3" s="53"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -3191,27 +3179,20 @@
         <v>23</v>
       </c>
       <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="H4" s="37">
+        <v>1</v>
+      </c>
       <c r="I4" s="37"/>
       <c r="J4" s="38" t="s">
         <v>45</v>
       </c>
       <c r="K4" s="39" t="str">
-        <f t="shared" ref="K4:K18" si="0">CONCATENATE(B4,CHAR(13),C4,CHAR(13),D4,CHAR(13),E4,CHAR(13),F4,CHAR(13),G4,CHAR(13),H4,CHAR(13),I4)</f>
-        <v>A_x000D_No_x000D_LC41_x000D_-_x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L4" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J4, SEARCH(",", J4, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_B1.fcs</v>
-      </c>
-      <c r="M4" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J4, SEARCH(",",J4) + 1, SEARCH(",",J4,SEARCH(",",J4)+1) - SEARCH(",",J4) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_B2.fcs</v>
-      </c>
-      <c r="N4" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J4,LEN(J4) - SEARCH(",", J4, SEARCH(",", J4) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_B3.fcs</v>
-      </c>
+        <f t="shared" ref="K4:K18" si="0">CONCATENATE(B4,CHAR(13),C4,CHAR(13),D4,CHAR(13),E4,CHAR(13),F4)</f>
+        <v>A_x000D_No_x000D_LC41_x000D_-_x000D_6 hrs</v>
+      </c>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
       <c r="O4" s="53"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3235,27 +3216,20 @@
         <v>23</v>
       </c>
       <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="H5" s="37">
+        <v>1</v>
+      </c>
       <c r="I5" s="37"/>
       <c r="J5" s="38" t="s">
         <v>47</v>
       </c>
       <c r="K5" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>B_x000D_No_x000D_LC41_x000D_-_x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L5" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J5, SEARCH(",", J5, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_C1.fcs</v>
-      </c>
-      <c r="M5" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J5, SEARCH(",",J5) + 1, SEARCH(",",J5,SEARCH(",",J5)+1) - SEARCH(",",J5) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_C2.fcs</v>
-      </c>
-      <c r="N5" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J5,LEN(J5) - SEARCH(",", J5, SEARCH(",", J5) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_C3.fcs</v>
-      </c>
+        <v>B_x000D_No_x000D_LC41_x000D_-_x000D_6 hrs</v>
+      </c>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
       <c r="O5" s="53"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -3279,27 +3253,20 @@
         <v>23</v>
       </c>
       <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="H6" s="37">
+        <v>1</v>
+      </c>
       <c r="I6" s="37"/>
       <c r="J6" s="38" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>C_x000D_No_x000D_LC20_x000D_-_x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L6" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J6, SEARCH(",", J6, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_D1.fcs</v>
-      </c>
-      <c r="M6" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J6, SEARCH(",",J6) + 1, SEARCH(",",J6,SEARCH(",",J6)+1) - SEARCH(",",J6) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_D2.fcs</v>
-      </c>
-      <c r="N6" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J6,LEN(J6) - SEARCH(",", J6, SEARCH(",", J6) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_D3.fcs</v>
-      </c>
+        <v>C_x000D_No_x000D_LC20_x000D_-_x000D_6 hrs</v>
+      </c>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
       <c r="O6" s="53"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -3323,27 +3290,20 @@
         <v>23</v>
       </c>
       <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="H7" s="37">
+        <v>1</v>
+      </c>
       <c r="I7" s="37"/>
       <c r="J7" s="38" t="s">
         <v>49</v>
       </c>
       <c r="K7" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>D_x000D_No_x000D_LC20_x000D_-_x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L7" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J7, SEARCH(",", J7, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_E1.fcs</v>
-      </c>
-      <c r="M7" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J7, SEARCH(",",J7) + 1, SEARCH(",",J7,SEARCH(",",J7)+1) - SEARCH(",",J7) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_E2.fcs</v>
-      </c>
-      <c r="N7" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J7,LEN(J7) - SEARCH(",", J7, SEARCH(",", J7) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_E3.fcs</v>
-      </c>
+        <v>D_x000D_No_x000D_LC20_x000D_-_x000D_6 hrs</v>
+      </c>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
       <c r="O7" s="53"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -3367,27 +3327,20 @@
         <v>23</v>
       </c>
       <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
+      <c r="H8" s="37">
+        <v>1</v>
+      </c>
       <c r="I8" s="37"/>
       <c r="J8" s="38" t="s">
         <v>50</v>
       </c>
       <c r="K8" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>X_x000D_No_x000D_-_x000D_+_x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L8" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J8, SEARCH(",", J8, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_F1.fcs</v>
-      </c>
-      <c r="M8" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J8, SEARCH(",",J8) + 1, SEARCH(",",J8,SEARCH(",",J8)+1) - SEARCH(",",J8) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_F2.fcs</v>
-      </c>
-      <c r="N8" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J8,LEN(J8) - SEARCH(",", J8, SEARCH(",", J8) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_F3.fcs</v>
-      </c>
+        <v>X_x000D_No_x000D_-_x000D_+_x000D_6 hrs</v>
+      </c>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
       <c r="O8" s="53"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -3411,27 +3364,20 @@
         <v>23</v>
       </c>
       <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
+      <c r="H9" s="37">
+        <v>1</v>
+      </c>
       <c r="I9" s="37"/>
       <c r="J9" s="38" t="s">
         <v>51</v>
       </c>
       <c r="K9" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>A_x000D_No_x000D_LC41_x000D_+_x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L9" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J9, SEARCH(",", J9, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_G1.fcs</v>
-      </c>
-      <c r="M9" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J9, SEARCH(",",J9) + 1, SEARCH(",",J9,SEARCH(",",J9)+1) - SEARCH(",",J9) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_G2.fcs</v>
-      </c>
-      <c r="N9" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J9,LEN(J9) - SEARCH(",", J9, SEARCH(",", J9) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_G3.fcs</v>
-      </c>
+        <v>A_x000D_No_x000D_LC41_x000D_+_x000D_6 hrs</v>
+      </c>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
       <c r="O9" s="53"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -3455,27 +3401,20 @@
         <v>23</v>
       </c>
       <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="H10" s="37">
+        <v>1</v>
+      </c>
       <c r="I10" s="37"/>
       <c r="J10" s="38" t="s">
         <v>52</v>
       </c>
       <c r="K10" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>B_x000D_No_x000D_LC41_x000D_+_x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L10" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J10, SEARCH(",", J10, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_H1.fcs</v>
-      </c>
-      <c r="M10" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J10, SEARCH(",",J10) + 1, SEARCH(",",J10,SEARCH(",",J10)+1) - SEARCH(",",J10) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_H2.fcs</v>
-      </c>
-      <c r="N10" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J10,LEN(J10) - SEARCH(",", J10, SEARCH(",", J10) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_H3.fcs</v>
-      </c>
+        <v>B_x000D_No_x000D_LC41_x000D_+_x000D_6 hrs</v>
+      </c>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
       <c r="O10" s="53"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -3499,27 +3438,20 @@
         <v>23</v>
       </c>
       <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="H11" s="37">
+        <v>1</v>
+      </c>
       <c r="I11" s="37"/>
       <c r="J11" s="38" t="s">
         <v>53</v>
       </c>
       <c r="K11" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>C_x000D_No_x000D_LC20_x000D_+_x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L11" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J11, SEARCH(",", J11, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_A4.fcs</v>
-      </c>
-      <c r="M11" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J11, SEARCH(",",J11) + 1, SEARCH(",",J11,SEARCH(",",J11)+1) - SEARCH(",",J11) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_A5.fcs</v>
-      </c>
-      <c r="N11" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J11,LEN(J11) - SEARCH(",", J11, SEARCH(",", J11) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_A6.fcs</v>
-      </c>
+        <v>C_x000D_No_x000D_LC20_x000D_+_x000D_6 hrs</v>
+      </c>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
       <c r="O11" s="53"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -3543,27 +3475,20 @@
         <v>23</v>
       </c>
       <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="H12" s="37">
+        <v>1</v>
+      </c>
       <c r="I12" s="37"/>
       <c r="J12" s="38" t="s">
         <v>54</v>
       </c>
       <c r="K12" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>D_x000D_No_x000D_LC20_x000D_+_x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L12" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J12, SEARCH(",", J12, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_B4.fcs</v>
-      </c>
-      <c r="M12" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J12, SEARCH(",",J12) + 1, SEARCH(",",J12,SEARCH(",",J12)+1) - SEARCH(",",J12) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_B5.fcs</v>
-      </c>
-      <c r="N12" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J12,LEN(J12) - SEARCH(",", J12, SEARCH(",", J12) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_B6.fcs</v>
-      </c>
+        <v>D_x000D_No_x000D_LC20_x000D_+_x000D_6 hrs</v>
+      </c>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
       <c r="O12" s="53"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -3581,27 +3506,20 @@
         <v>23</v>
       </c>
       <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="H13" s="37">
+        <v>1</v>
+      </c>
       <c r="I13" s="37"/>
       <c r="J13" s="38" t="s">
         <v>55</v>
       </c>
       <c r="K13" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>Blank_x000D__x000D__x000D__x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L13" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J13, SEARCH(",", J13, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_C4.fcs</v>
-      </c>
-      <c r="M13" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J13, SEARCH(",",J13) + 1, SEARCH(",",J13,SEARCH(",",J13)+1) - SEARCH(",",J13) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_C5.fcs</v>
-      </c>
-      <c r="N13" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J13,LEN(J13) - SEARCH(",", J13, SEARCH(",", J13) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_C6.fcs</v>
-      </c>
+        <v>Blank_x000D__x000D__x000D__x000D_6 hrs</v>
+      </c>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
       <c r="O13" s="53" t="s">
         <v>20</v>
       </c>
@@ -3621,27 +3539,20 @@
         <v>23</v>
       </c>
       <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
+      <c r="H14" s="37">
+        <v>1</v>
+      </c>
       <c r="I14" s="37"/>
       <c r="J14" s="38" t="s">
         <v>56</v>
       </c>
       <c r="K14" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>GFP_x000D__x000D__x000D__x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L14" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J14, SEARCH(",", J14, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_D4.fcs</v>
-      </c>
-      <c r="M14" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J14, SEARCH(",",J14) + 1, SEARCH(",",J14,SEARCH(",",J14)+1) - SEARCH(",",J14) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_D5.fcs</v>
-      </c>
-      <c r="N14" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J14,LEN(J14) - SEARCH(",", J14, SEARCH(",", J14) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_D6.fcs</v>
-      </c>
+        <v>GFP_x000D__x000D__x000D__x000D_6 hrs</v>
+      </c>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
       <c r="O14" s="53" t="s">
         <v>20</v>
       </c>
@@ -3661,27 +3572,20 @@
         <v>23</v>
       </c>
       <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
+      <c r="H15" s="37">
+        <v>1</v>
+      </c>
       <c r="I15" s="37"/>
       <c r="J15" s="38" t="s">
         <v>57</v>
       </c>
       <c r="K15" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>mRuby_x000D__x000D__x000D__x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L15" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J15, SEARCH(",", J15, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_E4.fcs</v>
-      </c>
-      <c r="M15" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J15, SEARCH(",",J15) + 1, SEARCH(",",J15,SEARCH(",",J15)+1) - SEARCH(",",J15) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_E5.fcs</v>
-      </c>
-      <c r="N15" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J15,LEN(J15) - SEARCH(",", J15, SEARCH(",", J15) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_E6.fcs</v>
-      </c>
+        <v>mRuby_x000D__x000D__x000D__x000D_6 hrs</v>
+      </c>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
       <c r="O15" s="53" t="s">
         <v>20</v>
       </c>
@@ -3701,27 +3605,20 @@
         <v>23</v>
       </c>
       <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
+      <c r="H16" s="37">
+        <v>1</v>
+      </c>
       <c r="I16" s="37"/>
       <c r="J16" s="38" t="s">
         <v>58</v>
       </c>
       <c r="K16" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>BFP_x000D__x000D__x000D__x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L16" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J16, SEARCH(",", J16, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_F4.fcs</v>
-      </c>
-      <c r="M16" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J16, SEARCH(",",J16) + 1, SEARCH(",",J16,SEARCH(",",J16)+1) - SEARCH(",",J16) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_F5.fcs</v>
-      </c>
-      <c r="N16" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J16,LEN(J16) - SEARCH(",", J16, SEARCH(",", J16) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_F6.fcs</v>
-      </c>
+        <v>BFP_x000D__x000D__x000D__x000D_6 hrs</v>
+      </c>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
       <c r="O16" s="53" t="s">
         <v>20</v>
       </c>
@@ -3741,27 +3638,20 @@
         <v>23</v>
       </c>
       <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
+      <c r="H17" s="37">
+        <v>1</v>
+      </c>
       <c r="I17" s="37"/>
       <c r="J17" s="38" t="s">
         <v>59</v>
       </c>
       <c r="K17" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>All_x000D__x000D__x000D__x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L17" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J17, SEARCH(",", J17, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_G4.fcs</v>
-      </c>
-      <c r="M17" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J17, SEARCH(",",J17) + 1, SEARCH(",",J17,SEARCH(",",J17)+1) - SEARCH(",",J17) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_G5.fcs</v>
-      </c>
-      <c r="N17" s="40" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J17,LEN(J17) - SEARCH(",", J17, SEARCH(",", J17) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_G6.fcs</v>
-      </c>
+        <v>All_x000D__x000D__x000D__x000D_6 hrs</v>
+      </c>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
       <c r="O17" s="53" t="s">
         <v>20</v>
       </c>
@@ -3781,27 +3671,20 @@
         <v>23</v>
       </c>
       <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
+      <c r="H18" s="42">
+        <v>1</v>
+      </c>
       <c r="I18" s="42"/>
       <c r="J18" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="K18" s="107" t="str">
+      <c r="K18" s="155" t="str">
         <f t="shared" si="0"/>
-        <v>Beads_x000D__x000D__x000D__x000D_6 hrs_x000D__x000D__x000D_</v>
-      </c>
-      <c r="L18" s="44" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",LEFT(J18, SEARCH(",", J18, 1)-1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_H4.fcs</v>
-      </c>
-      <c r="M18" s="44" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",MID(J18, SEARCH(",",J18) + 1, SEARCH(",",J18,SEARCH(",",J18)+1) - SEARCH(",",J18) - 1),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_H5.fcs</v>
-      </c>
-      <c r="N18" s="44" t="str">
-        <f>CONCATENATE(Experiment!$A$4,"_",20180429,"_Group1","_Plate1","_",RIGHT(J18,LEN(J18) - SEARCH(",", J18, SEARCH(",", J18) + 1)),".fcs")</f>
-        <v>JHT2_20180429_Group1_Plate1_H6.fcs</v>
-      </c>
+        <v>Beads_x000D__x000D__x000D__x000D_6 hrs</v>
+      </c>
+      <c r="L18" s="44"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="44"/>
       <c r="O18" s="54" t="s">
         <v>20</v>
       </c>
@@ -3821,91 +3704,93 @@
       <c r="I20" s="150"/>
       <c r="J20" s="151"/>
     </row>
-    <row r="21" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="152" t="s">
+    <row r="22" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N22" s="111"/>
+    </row>
+    <row r="25" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="152" t="s">
         <v>230</v>
       </c>
-      <c r="C22" s="153"/>
-      <c r="D22" s="153"/>
-      <c r="E22" s="153"/>
-      <c r="F22" s="153"/>
-      <c r="G22" s="153"/>
-      <c r="H22" s="153"/>
-      <c r="I22" s="153"/>
-      <c r="J22" s="153"/>
-      <c r="K22" s="153"/>
-      <c r="L22" s="153"/>
-      <c r="M22" s="154"/>
-      <c r="N22" s="112"/>
-    </row>
-    <row r="23" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="B23" s="104" t="s">
+      <c r="C26" s="153"/>
+      <c r="D26" s="153"/>
+      <c r="E26" s="153"/>
+      <c r="F26" s="153"/>
+      <c r="G26" s="153"/>
+      <c r="H26" s="153"/>
+      <c r="I26" s="153"/>
+      <c r="J26" s="153"/>
+      <c r="K26" s="153"/>
+      <c r="L26" s="153"/>
+      <c r="M26" s="154"/>
+    </row>
+    <row r="27" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="B27" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="106" t="s">
+      <c r="C27" s="106" t="s">
         <v>258</v>
       </c>
-      <c r="D23" s="106" t="s">
+      <c r="D27" s="106" t="s">
         <v>257</v>
       </c>
-      <c r="E23" s="106" t="s">
+      <c r="E27" s="106" t="s">
         <v>231</v>
       </c>
-      <c r="F23" s="106" t="s">
+      <c r="F27" s="106" t="s">
         <v>164</v>
       </c>
-      <c r="G23" s="106" t="s">
+      <c r="G27" s="106" t="s">
         <v>165</v>
       </c>
-      <c r="H23" s="106" t="s">
+      <c r="H27" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="I23" s="106" t="s">
+      <c r="I27" s="106" t="s">
         <v>232</v>
       </c>
-      <c r="J23" s="106" t="s">
+      <c r="J27" s="106" t="s">
         <v>233</v>
       </c>
-      <c r="K23" s="106" t="s">
+      <c r="K27" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="L23" s="106"/>
-      <c r="M23" s="111"/>
-    </row>
-    <row r="24" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="108" t="s">
+      <c r="L27" s="106"/>
+      <c r="M27" s="110"/>
+    </row>
+    <row r="28" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="107" t="s">
         <v>261</v>
       </c>
-      <c r="C24" s="115"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47">
+      <c r="C28" s="114"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47">
         <v>100</v>
       </c>
-      <c r="G24" s="47">
+      <c r="G28" s="47">
         <v>0</v>
       </c>
-      <c r="H24" s="47">
+      <c r="H28" s="47">
         <v>0.6</v>
       </c>
-      <c r="I24" s="47">
+      <c r="I28" s="47">
         <v>4</v>
       </c>
-      <c r="J24" s="47">
+      <c r="J28" s="47">
         <v>10</v>
       </c>
-      <c r="K24" s="47">
+      <c r="K28" s="47">
         <v>10</v>
       </c>
-      <c r="L24" s="47"/>
-      <c r="M24" s="109"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="A20:J20"/>
-    <mergeCell ref="B22:M22"/>
+    <mergeCell ref="B26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>